<commit_message>
cap nhat giao dich theo breakout
</commit_message>
<xml_diff>
--- a/GiaoDichKhongCanPhanTich.xlsx
+++ b/GiaoDichKhongCanPhanTich.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Người thực hiện:</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Đặt take profit x2 lần giá từ đáy hình thành tới cái đỉnh đó</t>
   </si>
   <si>
-    <t>Cái này còn tùy từng cặp tiền tệ</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chờ đến khi giá phá cái đỉnh, sau đó có 1 cái nến đỏ xuất hiện, </t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>Khi giá quay trở về test cái đỉnh trước đó thì sẽ chờ một cái nến vàng hay nến pinbar hay mô hình nến đảo chiều xuất hiện</t>
   </si>
   <si>
-    <t>Sau khi nến vàng xuất hiện thì ta sẽ đặt lệnh buy và stoploss dưới cái nến đảo chiều đấy vài pip</t>
-  </si>
-  <si>
     <t>Tương tự với xu hướng giảm</t>
   </si>
   <si>
@@ -231,13 +225,37 @@
     <t>ví dụ như ở vùng 1 thì ta vẫn nên chờ khi giá phá qua ngưỡng 6 thì sẽ trở lại ngưỡng 5 rồi tiếp diễn xu hướng</t>
   </si>
   <si>
-    <t>còn ở vùng 2 thì số pip quá lớn nên khả năng đảo chiều rất cao</t>
-  </si>
-  <si>
     <t>Donate USDT Binance Smart Chain (BEP20)</t>
   </si>
   <si>
     <t>0xed05b97f46e60a7a65605eaba9a4b502d32f9510</t>
+  </si>
+  <si>
+    <t>nhiều khi chưa chắc giá đã về đỉnh trước đo mà đã đi tiếp</t>
+  </si>
+  <si>
+    <t>Sau khi nến đảo chiều xuất hiện thì ta sẽ đặt lệnh buy và stoploss dưới cái nến đảo chiều đấy vài pip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">khả năng có nến vàng rất cao hoặc nó xuống vài nến đỏ </t>
+  </si>
+  <si>
+    <t>nhưng chắc chắn sẽ retest lại cái vùng đỉnh trước đó</t>
+  </si>
+  <si>
+    <t>Quy luật xu hướng mạnh, yếu</t>
+  </si>
+  <si>
+    <t>Phải hiểu được sự mạnh, yếu thì mới biết được thị trường sẽ dịch chuyển như thế nào</t>
+  </si>
+  <si>
+    <t>Nến có râu nằm trên ngưỡng không được thừa nhận</t>
+  </si>
+  <si>
+    <t>Khi vùng 1 xuất hiện thì hãy cẩn thận do cho dù giá có cao hơn nữa thì khả năng đảo chiều rất cao do cho thấy lực bán mạnh đã xuất hiện</t>
+  </si>
+  <si>
+    <t>còn ở vùng 2 thì số pip quá lớn nên nếu phá vỡ thì khả năng đảo chiều rất cao</t>
   </si>
 </sst>
 </file>
@@ -331,13 +349,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4762</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>376237</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -648,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T114"/>
+  <dimension ref="A1:P126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="C109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M128" sqref="M128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,13 +806,13 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -830,7 +848,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -838,7 +856,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>12</v>
       </c>
@@ -846,17 +864,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>17</v>
       </c>
@@ -864,255 +882,283 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>74</v>
+      </c>
+      <c r="I28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="67" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C67" t="s">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="F72" t="s">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="F73" t="s">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="F74" t="s">
+    <row r="81" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
         <v>28</v>
       </c>
-      <c r="J74" t="s">
+      <c r="G81" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="J75" t="s">
+    <row r="82" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="G82" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="76" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="J76" t="s">
+      <c r="O82" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="83" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="G83" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="84" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="G84" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="85" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="G85" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="86" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="H86" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="87" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="H87">
+        <v>1</v>
+      </c>
+      <c r="I87" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="88" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="H88">
+        <v>2</v>
+      </c>
+      <c r="I88" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="89" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="H89">
+        <v>3</v>
+      </c>
+      <c r="I89" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="90" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="I90" t="s">
+        <v>35</v>
+      </c>
+      <c r="O90" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="91" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O91" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="93" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="H93">
+        <v>4</v>
+      </c>
+      <c r="I93" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="94" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="G94" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="77" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="J77" t="s">
+    <row r="96" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="78" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="J78" t="s">
-        <v>31</v>
-      </c>
-      <c r="M78" t="s">
+    <row r="98" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="99" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="101" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="103" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>42</v>
+      </c>
+      <c r="M103" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="104" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>43</v>
+      </c>
+      <c r="M104" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="108" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D108" t="s">
+        <v>46</v>
+      </c>
+      <c r="F108" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="109" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="F109" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="110" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="F110" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="111" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="F111" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="112" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="F112" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="113" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F113" t="s">
+        <v>51</v>
+      </c>
+      <c r="I113" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="114" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="I114" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="116" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F116" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="118" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="G118" t="s">
+        <v>56</v>
+      </c>
+      <c r="I118" t="s">
+        <v>55</v>
+      </c>
+      <c r="L118" t="s">
+        <v>59</v>
+      </c>
+      <c r="P118" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="119" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="G119" t="s">
+        <v>57</v>
+      </c>
+      <c r="I119" t="s">
+        <v>58</v>
+      </c>
+      <c r="L119" t="s">
+        <v>60</v>
+      </c>
+      <c r="P119" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="121" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F121" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="79" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="M79">
-        <v>1</v>
-      </c>
-      <c r="N79" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="80" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="M80">
-        <v>2</v>
-      </c>
-      <c r="N80" t="s">
-        <v>33</v>
-      </c>
-      <c r="T80" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="81" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="M81">
-        <v>3</v>
-      </c>
-      <c r="N81" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="82" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="N82" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="83" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="M83">
-        <v>4</v>
-      </c>
-      <c r="N83" s="6" t="s">
+    <row r="122" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="G122" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="84" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="J84" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="86" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C86" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="88" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D88" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="89" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D89" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="91" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D91" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="93" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="E93" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q93" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="94" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="E94" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q94" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="98" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D98" t="s">
-        <v>48</v>
-      </c>
-      <c r="F98" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="100" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="F100" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="101" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="F101" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="102" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="F102" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="103" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="F103" t="s">
-        <v>53</v>
-      </c>
-      <c r="I103" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="104" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="I104" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="106" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="F106" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="108" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="G108" t="s">
-        <v>58</v>
-      </c>
-      <c r="I108" t="s">
-        <v>57</v>
-      </c>
-      <c r="L108" t="s">
-        <v>61</v>
-      </c>
-      <c r="P108" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="109" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="G109" t="s">
-        <v>59</v>
-      </c>
-      <c r="I109" t="s">
-        <v>60</v>
-      </c>
-      <c r="L109" t="s">
-        <v>62</v>
-      </c>
-      <c r="P109" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="111" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="F111" t="s">
+    <row r="123" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="G123" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="112" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="G112" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="113" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G113" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="114" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G114" t="s">
-        <v>70</v>
+    <row r="124" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="G124" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="126" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="G126" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>